<commit_message>
serilizer not finished yet
</commit_message>
<xml_diff>
--- a/report/static/excel/detail.xlsx
+++ b/report/static/excel/detail.xlsx
@@ -441,72 +441,72 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>user</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>dsc</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>district_status</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>state_status</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>central_status</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>private_status</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>approved_pending_cancelled</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>created_at</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>updated_at</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>is_payment</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>bill_number</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>payment_get</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>type_application_id</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>get_user_application_detail</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>user</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
@@ -532,13 +532,13 @@
       <c r="B2" t="n">
         <v>23</v>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" t="n">
+        <v>40</v>
+      </c>
+      <c r="D2" t="inlineStr">
         <is>
           <t>central_admin</t>
         </is>
-      </c>
-      <c r="D2" t="b">
-        <v>0</v>
       </c>
       <c r="E2" t="b">
         <v>0</v>
@@ -549,44 +549,44 @@
       <c r="G2" t="b">
         <v>0</v>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="H2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>2022-11-29T11:40:29.878938+05:45</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>2022-11-30T13:21:07.217079+05:45</t>
-        </is>
-      </c>
-      <c r="K2" t="b">
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>2022-11-30T13:26:43.523007+05:45</t>
+        </is>
+      </c>
+      <c r="L2" t="b">
         <v>1</v>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="M2" t="inlineStr">
         <is>
           <t>234234</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="N2" t="inlineStr">
         <is>
           <t>234234</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="O2" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="O2" t="n">
+      <c r="P2" t="n">
         <v>23</v>
-      </c>
-      <c r="P2" t="n">
-        <v>40</v>
       </c>
       <c r="Q2" t="inlineStr"/>
       <c r="R2" t="inlineStr"/>

</xml_diff>